<commit_message>
reimplemented the tests with correct url
</commit_message>
<xml_diff>
--- a/Midterm-exam/evidence/spreadsheets/per_site/www.as.kommune.no.xlsx
+++ b/Midterm-exam/evidence/spreadsheets/per_site/www.as.kommune.no.xlsx
@@ -445,31 +445,31 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>8837.937999999998</v>
+        <v>8675.0985</v>
       </c>
       <c r="C2">
-        <v>4237.936</v>
+        <v>4412.286999999999</v>
       </c>
       <c r="D2">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E2">
-        <v>8877.077949999999</v>
+        <v>9791.44360366974</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <v>0.0009715726896401236</v>
       </c>
       <c r="H2">
-        <v>4237.936</v>
+        <v>4412.286999999999</v>
       </c>
       <c r="I2">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J2">
-        <v>1537160</v>
+        <v>1521124</v>
       </c>
       <c r="K2">
         <v>47</v>
@@ -480,16 +480,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>10544.154821517943</v>
+        <v>8864.754</v>
       </c>
       <c r="C3">
-        <v>5888.84275</v>
+        <v>3999.3625</v>
       </c>
       <c r="D3">
         <v>26</v>
       </c>
       <c r="E3">
-        <v>10622.462003669738</v>
+        <v>8911.6473</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -498,13 +498,13 @@
         <v>0.0009715726896401236</v>
       </c>
       <c r="H3">
-        <v>5888.84275</v>
+        <v>3999.3625</v>
       </c>
       <c r="I3">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="J3">
-        <v>1537129</v>
+        <v>1521144</v>
       </c>
       <c r="K3">
         <v>47</v>
@@ -515,16 +515,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>8959.0615</v>
+        <v>8696.737000000001</v>
       </c>
       <c r="C4">
-        <v>4244.109</v>
+        <v>3947.6630000000005</v>
       </c>
       <c r="D4">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4">
-        <v>8998.73515</v>
+        <v>8751.6296</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -533,13 +533,13 @@
         <v>0.0009715726896401236</v>
       </c>
       <c r="H4">
-        <v>4244.109</v>
+        <v>3947.6630000000005</v>
       </c>
       <c r="I4">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J4">
-        <v>1537136</v>
+        <v>1521130</v>
       </c>
       <c r="K4">
         <v>47</v>
@@ -550,16 +550,16 @@
         <v>median</v>
       </c>
       <c r="B5">
-        <v>8959.0615</v>
+        <v>8696.737000000001</v>
       </c>
       <c r="C5">
-        <v>4244.109</v>
+        <v>3999.3625</v>
       </c>
       <c r="D5">
         <v>27</v>
       </c>
       <c r="E5">
-        <v>8998.73515</v>
+        <v>8911.6473</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -568,13 +568,13 @@
         <v>0.0009715726896401236</v>
       </c>
       <c r="H5">
-        <v>4244.109</v>
+        <v>3999.3625</v>
       </c>
       <c r="I5">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J5">
-        <v>1537136</v>
+        <v>1521130</v>
       </c>
       <c r="K5">
         <v>47</v>
@@ -634,16 +634,16 @@
         <v>text/html</v>
       </c>
       <c r="E2">
-        <v>31231</v>
+        <v>31258</v>
       </c>
       <c r="F2">
-        <v>154090</v>
+        <v>153996</v>
       </c>
       <c r="G2">
-        <v>0.009082380802999999</v>
+        <v>0.009090232753999998</v>
       </c>
       <c r="H2">
-        <v>0.011964015203400003</v>
+        <v>0.011974358401200003</v>
       </c>
     </row>
     <row r="3">
@@ -712,16 +712,16 @@
         <v>text/css</v>
       </c>
       <c r="E5">
-        <v>60280</v>
+        <v>60279</v>
       </c>
       <c r="F5">
         <v>599332</v>
       </c>
       <c r="G5">
-        <v>0.017530207639999996</v>
+        <v>0.017529916826999996</v>
       </c>
       <c r="H5">
-        <v>0.023092146792000005</v>
+        <v>0.0230917637106</v>
       </c>
     </row>
     <row r="6">
@@ -738,16 +738,16 @@
         <v>text/css</v>
       </c>
       <c r="E6">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F6">
         <v>578</v>
       </c>
       <c r="G6">
-        <v>0.000171870483</v>
+        <v>0.00017157967</v>
       </c>
       <c r="H6">
-        <v>0.00022640110740000002</v>
+        <v>0.00022601802599999998</v>
       </c>
     </row>
     <row r="7">
@@ -764,16 +764,16 @@
         <v>text/css</v>
       </c>
       <c r="E7">
-        <v>2226</v>
+        <v>2227</v>
       </c>
       <c r="F7">
         <v>17559</v>
       </c>
       <c r="G7">
-        <v>0.0006473497379999998</v>
+        <v>0.0006476405509999999</v>
       </c>
       <c r="H7">
-        <v>0.0008527391964</v>
+        <v>0.0008531222778000001</v>
       </c>
     </row>
     <row r="8">
@@ -790,16 +790,16 @@
         <v>text/css</v>
       </c>
       <c r="E8">
-        <v>3484</v>
+        <v>3483</v>
       </c>
       <c r="F8">
         <v>12189</v>
       </c>
       <c r="G8">
-        <v>0.0010131924919999998</v>
+        <v>0.001012901679</v>
       </c>
       <c r="H8">
-        <v>0.0013346555976</v>
+        <v>0.0013342725162000001</v>
       </c>
     </row>
     <row r="9">
@@ -842,16 +842,16 @@
         <v>text/javascript</v>
       </c>
       <c r="E10">
-        <v>89995</v>
+        <v>31287</v>
       </c>
       <c r="F10">
         <v>89664</v>
       </c>
       <c r="G10">
-        <v>0.026171715934999996</v>
+        <v>0.009098666330999998</v>
       </c>
       <c r="H10">
-        <v>0.034475410593</v>
+        <v>0.011985467761800001</v>
       </c>
     </row>
     <row r="11">
@@ -885,7 +885,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="str">
-        <v>https://www.as.kommune.no/css/cpcommon.css?v=20251110</v>
+        <v>https://www.as.kommune.no/css/cpcommon.css?v=20251114</v>
       </c>
       <c r="C12" t="str">
         <v>Stylesheet</v>
@@ -1015,7 +1015,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464727.2703.jkzawaluazsnml/660f450/0_5464727.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5465224.2703.77iqmqbjzltqtt/660f450/0_5465224.jpg</v>
       </c>
       <c r="C17" t="str">
         <v>Image</v>
@@ -1024,16 +1024,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E17">
-        <v>43748</v>
+        <v>41979</v>
       </c>
       <c r="F17">
-        <v>43380</v>
+        <v>41611</v>
       </c>
       <c r="G17">
-        <v>0.012722487123999999</v>
+        <v>0.012208038926999999</v>
       </c>
       <c r="H17">
-        <v>0.0167590450872</v>
+        <v>0.0160813740906</v>
       </c>
     </row>
     <row r="18">
@@ -1041,7 +1041,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464715.2703.bpjzpuutzsii7i/660f450/0_5464715.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5308658.2703.aabaszjkaptpbb/660f450/0_5308658.jpg</v>
       </c>
       <c r="C18" t="str">
         <v>Image</v>
@@ -1050,16 +1050,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E18">
-        <v>66510</v>
+        <v>29106</v>
       </c>
       <c r="F18">
-        <v>66142</v>
+        <v>28738</v>
       </c>
       <c r="G18">
-        <v>0.019341972629999996</v>
+        <v>0.008464403177999999</v>
       </c>
       <c r="H18">
-        <v>0.025478743914000006</v>
+        <v>0.011149967228399999</v>
       </c>
     </row>
     <row r="19">
@@ -1067,25 +1067,25 @@
         <v>1</v>
       </c>
       <c r="B19" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464624.2703.miqqnuwwzzswqt/660f450/0_5464624.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5464874.2703.jblqzspatzuwkt/660f450/0_5464874.png</v>
       </c>
       <c r="C19" t="str">
         <v>Image</v>
       </c>
       <c r="D19" t="str">
-        <v>image/jpeg</v>
+        <v>image/png</v>
       </c>
       <c r="E19">
-        <v>43585</v>
+        <v>159684</v>
       </c>
       <c r="F19">
-        <v>43217</v>
+        <v>159316</v>
       </c>
       <c r="G19">
-        <v>0.012675084605</v>
+        <v>0.046438183092</v>
       </c>
       <c r="H19">
-        <v>0.016696602819</v>
+        <v>0.061171970277600005</v>
       </c>
     </row>
     <row r="20">
@@ -1093,7 +1093,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464266.2703.tkumwmpjsjqllz/660f450/0_5464266.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5464727.2703.jkzawaluazsnml/660f450/0_5464727.jpg</v>
       </c>
       <c r="C20" t="str">
         <v>Image</v>
@@ -1102,16 +1102,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E20">
-        <v>50396</v>
+        <v>43748</v>
       </c>
       <c r="F20">
-        <v>50028</v>
+        <v>43380</v>
       </c>
       <c r="G20">
-        <v>0.014655811947999997</v>
+        <v>0.012722487123999999</v>
       </c>
       <c r="H20">
-        <v>0.019305770234400003</v>
+        <v>0.0167590450872</v>
       </c>
     </row>
     <row r="21">
@@ -1119,7 +1119,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464265.2703.jakzlmuauupstp/660f450/0_5464265.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5464715.2703.bpjzpuutzsii7i/660f450/0_5464715.jpg</v>
       </c>
       <c r="C21" t="str">
         <v>Image</v>
@@ -1128,16 +1128,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E21">
-        <v>40520</v>
+        <v>66510</v>
       </c>
       <c r="F21">
-        <v>40152</v>
+        <v>66142</v>
       </c>
       <c r="G21">
-        <v>0.011783742759999999</v>
+        <v>0.019341972629999996</v>
       </c>
       <c r="H21">
-        <v>0.015522458328000002</v>
+        <v>0.025478743914000006</v>
       </c>
     </row>
     <row r="22">
@@ -1145,7 +1145,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464165.2703.njinmipitzqa7i/660f450/0_5464165.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5464624.2703.miqqnuwwzzswqt/660f450/0_5464624.jpg</v>
       </c>
       <c r="C22" t="str">
         <v>Image</v>
@@ -1154,16 +1154,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E22">
-        <v>61382</v>
+        <v>43585</v>
       </c>
       <c r="F22">
-        <v>61014</v>
+        <v>43217</v>
       </c>
       <c r="G22">
-        <v>0.017850683565999996</v>
+        <v>0.012675084605</v>
       </c>
       <c r="H22">
-        <v>0.023514302494800004</v>
+        <v>0.016696602819</v>
       </c>
     </row>
     <row r="23">
@@ -1171,7 +1171,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="str">
-        <v>https://media.newmindmedia.com/TellUs/image/?file=Bilde_av_plakat_4__2060226217.png&amp;dh=515&amp;dw=350</v>
+        <v>https://media.newmindmedia.com/TellUs/image/?file=Logo_A_s_JPG_2__1509348857.jpg&amp;dh=139&amp;dw=350</v>
       </c>
       <c r="C23" t="str">
         <v>Image</v>
@@ -1180,16 +1180,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E23">
-        <v>47261</v>
+        <v>8692</v>
       </c>
       <c r="F23">
-        <v>46939</v>
+        <v>8414</v>
       </c>
       <c r="G23">
-        <v>0.013744113192999998</v>
+        <v>0.0025277465959999998</v>
       </c>
       <c r="H23">
-        <v>0.018104810045400002</v>
+        <v>0.0033297435288000008</v>
       </c>
     </row>
     <row r="24">
@@ -1197,7 +1197,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="str">
-        <v>https://media.newmindmedia.com/TellUs/image/?file=Vintersykkelfest_233473079.jpg&amp;dh=350&amp;dw=350</v>
+        <v>https://media.newmindmedia.com/TellUs/image/?file=F322105710F853B986D230AE1BF4B921F4143F8C_944246711.jpg&amp;dh=361&amp;dw=350</v>
       </c>
       <c r="C24" t="str">
         <v>Image</v>
@@ -1206,16 +1206,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E24">
-        <v>33726</v>
+        <v>26125</v>
       </c>
       <c r="F24">
-        <v>33422</v>
+        <v>25830</v>
       </c>
       <c r="G24">
-        <v>0.009807959237999998</v>
+        <v>0.007597489624999999</v>
       </c>
       <c r="H24">
-        <v>0.0129198032964</v>
+        <v>0.010008001575000001</v>
       </c>
     </row>
     <row r="25">
@@ -1223,7 +1223,7 @@
         <v>1</v>
       </c>
       <c r="B25" t="str">
-        <v>https://media.newmindmedia.com/TellUs/image/?file=KRED_1794052439.jpg&amp;dh=197&amp;dw=350</v>
+        <v>https://media.newmindmedia.com/TellUs/image/?file=1B4C24285867A1B7CDF44DF0370ACB0E18D8485A_1352853877.jpg&amp;dh=469&amp;dw=350</v>
       </c>
       <c r="C25" t="str">
         <v>Image</v>
@@ -1232,16 +1232,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E25">
-        <v>12203</v>
+        <v>22582</v>
       </c>
       <c r="F25">
-        <v>11924</v>
+        <v>22296</v>
       </c>
       <c r="G25">
-        <v>0.0035487910389999993</v>
+        <v>0.006567139165999999</v>
       </c>
       <c r="H25">
-        <v>0.0046747423242</v>
+        <v>0.008650744174800003</v>
       </c>
     </row>
     <row r="26">
@@ -1258,16 +1258,16 @@
         <v>application/javascript</v>
       </c>
       <c r="E26">
-        <v>13700</v>
+        <v>13688</v>
       </c>
       <c r="F26">
         <v>43534</v>
       </c>
       <c r="G26">
-        <v>0.0039841380999999995</v>
+        <v>0.003980648343999999</v>
       </c>
       <c r="H26">
-        <v>0.005248215180000001</v>
+        <v>0.0052436182032</v>
       </c>
     </row>
     <row r="27">
@@ -1388,16 +1388,16 @@
         <v>text/javascript</v>
       </c>
       <c r="E31">
-        <v>8420</v>
+        <v>8419</v>
       </c>
       <c r="F31">
-        <v>27186</v>
+        <v>27184</v>
       </c>
       <c r="G31">
-        <v>0.00244864546</v>
+        <v>0.002448354647</v>
       </c>
       <c r="H31">
-        <v>0.003225545388000001</v>
+        <v>0.0032251623066</v>
       </c>
     </row>
     <row r="32">
@@ -1405,25 +1405,25 @@
         <v>1</v>
       </c>
       <c r="B32" t="str">
-        <v>https://img6.custompublish.com/getfile.php/4236909.2316.bmupiw7su7pkam/search.svg</v>
+        <v>https://www.as.kommune.no/cpclass/run/sitefeedback/feedback.css.php</v>
       </c>
       <c r="C32" t="str">
-        <v>Image</v>
+        <v>Stylesheet</v>
       </c>
       <c r="D32" t="str">
-        <v>image/svg+xml</v>
+        <v>text/css</v>
       </c>
       <c r="E32">
-        <v>750</v>
+        <v>1467</v>
       </c>
       <c r="F32">
-        <v>384</v>
+        <v>4738</v>
       </c>
       <c r="G32">
-        <v>0.00021810974999999998</v>
+        <v>0.0004266226709999999</v>
       </c>
       <c r="H32">
-        <v>0.00028731105</v>
+        <v>0.0005619804138</v>
       </c>
     </row>
     <row r="33">
@@ -1431,22 +1431,25 @@
         <v>1</v>
       </c>
       <c r="B33" t="str">
-        <v>https://www.as.kommune.no/getfile.php/5223855.2703.mtbjbmbz7qptju/1280x0/nettsidebanner-ny-melkeveien.png</v>
+        <v>https://img6.custompublish.com/getfile.php/4236909.2316.bmupiw7su7pkam/search.svg</v>
       </c>
       <c r="C33" t="str">
-        <v>other</v>
+        <v>Image</v>
       </c>
       <c r="D33" t="str">
-        <v>text/html</v>
+        <v>image/svg+xml</v>
       </c>
       <c r="E33">
-        <v>310</v>
+        <v>750</v>
+      </c>
+      <c r="F33">
+        <v>384</v>
       </c>
       <c r="G33">
-        <v>0.00009015202999999999</v>
+        <v>0.00021810974999999998</v>
       </c>
       <c r="H33">
-        <v>0.00011875523400000001</v>
+        <v>0.00028731105</v>
       </c>
     </row>
     <row r="34">
@@ -1454,25 +1457,22 @@
         <v>1</v>
       </c>
       <c r="B34" t="str">
-        <v>https://fonts.gstatic.com/s/opensans/v44/memvYaGs126MiZpBA-UvWbX2vVnXBbObj2OVTS-mu0SC55I.woff2</v>
+        <v>https://www.as.kommune.no/getfile.php/5223855.2703.mtbjbmbz7qptju/1280x0/nettsidebanner-ny-melkeveien.png</v>
       </c>
       <c r="C34" t="str">
-        <v>Font</v>
+        <v>other</v>
       </c>
       <c r="D34" t="str">
-        <v>font/woff2</v>
+        <v>text/html</v>
       </c>
       <c r="E34">
-        <v>42996</v>
-      </c>
-      <c r="F34">
-        <v>42964</v>
+        <v>310</v>
       </c>
       <c r="G34">
-        <v>0.012503795747999999</v>
+        <v>0.00009015202999999999</v>
       </c>
       <c r="H34">
-        <v>0.0164709678744</v>
+        <v>0.00011875523400000001</v>
       </c>
     </row>
     <row r="35">
@@ -1480,25 +1480,25 @@
         <v>1</v>
       </c>
       <c r="B35" t="str">
-        <v>https://www.as.kommune.no/cpclass/css/scss-imports/v6.4.3/scss/icon-fonts/foundation-icon-fonts/foundation-icons.woff</v>
+        <v>https://fonts.gstatic.com/s/opensans/v44/memvYaGs126MiZpBA-UvWbX2vVnXBbObj2OVTS-mu0SC55I.woff2</v>
       </c>
       <c r="C35" t="str">
         <v>Font</v>
       </c>
       <c r="D35" t="str">
-        <v>font/woff</v>
+        <v>font/woff2</v>
       </c>
       <c r="E35">
-        <v>32294</v>
+        <v>42996</v>
       </c>
       <c r="F35">
-        <v>32020</v>
+        <v>42964</v>
       </c>
       <c r="G35">
-        <v>0.009391515021999999</v>
+        <v>0.012503795747999999</v>
       </c>
       <c r="H35">
-        <v>0.012371230731600001</v>
+        <v>0.0164709678744</v>
       </c>
     </row>
     <row r="36">
@@ -1506,25 +1506,25 @@
         <v>1</v>
       </c>
       <c r="B36" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5223855.2703.mtbjbmbz7qptju/1280x0/nettsidebanner-ny-melkeveien.png?return=www.as.kommune.no</v>
+        <v>https://www.as.kommune.no/cpclass/css/scss-imports/v6.4.3/scss/icon-fonts/foundation-icon-fonts/foundation-icons.woff</v>
       </c>
       <c r="C36" t="str">
-        <v>Image</v>
+        <v>Font</v>
       </c>
       <c r="D36" t="str">
-        <v>image/png</v>
+        <v>font/woff</v>
       </c>
       <c r="E36">
-        <v>232784</v>
+        <v>32294</v>
       </c>
       <c r="F36">
-        <v>232397</v>
+        <v>32020</v>
       </c>
       <c r="G36">
-        <v>0.06769661339199999</v>
+        <v>0.009391515021999999</v>
       </c>
       <c r="H36">
-        <v>0.08917522061760003</v>
+        <v>0.012371230731600001</v>
       </c>
     </row>
     <row r="37">
@@ -1532,25 +1532,25 @@
         <v>1</v>
       </c>
       <c r="B37" t="str">
-        <v>https://www.as.kommune.no/cpclass/run/sitefeedback/feedback.css.php</v>
+        <v>https://img3.custompublish.com/getfile.php/5223855.2703.mtbjbmbz7qptju/1280x0/nettsidebanner-ny-melkeveien.png?return=www.as.kommune.no</v>
       </c>
       <c r="C37" t="str">
-        <v>Stylesheet</v>
+        <v>Image</v>
       </c>
       <c r="D37" t="str">
-        <v>text/css</v>
+        <v>image/png</v>
       </c>
       <c r="E37">
-        <v>1467</v>
+        <v>232784</v>
       </c>
       <c r="F37">
-        <v>4738</v>
+        <v>232397</v>
       </c>
       <c r="G37">
-        <v>0.0004266226709999999</v>
+        <v>0.06769661339199999</v>
       </c>
       <c r="H37">
-        <v>0.0005619804138</v>
+        <v>0.08917522061760003</v>
       </c>
     </row>
     <row r="38">
@@ -1567,16 +1567,16 @@
         <v>text/html</v>
       </c>
       <c r="E38">
-        <v>4040</v>
+        <v>4039</v>
       </c>
       <c r="F38">
         <v>15600</v>
       </c>
       <c r="G38">
-        <v>0.0011748845199999998</v>
+        <v>0.0011745937069999998</v>
       </c>
       <c r="H38">
-        <v>0.0015476488560000005</v>
+        <v>0.0015472657746</v>
       </c>
     </row>
     <row r="39">
@@ -1636,7 +1636,7 @@
         <v>1</v>
       </c>
       <c r="B41" t="str">
-        <v>https://6002261.global.siteimproveanalytics.io/image.aspx?url=https%3A%2F%2Fwww.as.kommune.no%2F&amp;title=Forside%20-%20%C3%85S%20KOMMUNE&amp;res=412x823&amp;accountid=6002261&amp;rt=234&amp;prev=0d7cef22-22a6-8061-1040-a0c5f6f37df9&amp;luid=bb168c19-4de6-4061-798f-8d0dd129af8e&amp;rnd=70101</v>
+        <v>https://6002261.global.siteimproveanalytics.io/image.aspx?url=https%3A%2F%2Fwww.as.kommune.no%2F&amp;title=Forside%20-%20%C3%85S%20KOMMUNE&amp;res=412x823&amp;accountid=6002261&amp;rt=260&amp;prev=1e7a0237-4d46-092f-8145-fb29126daf21&amp;luid=eb023062-4ac4-3346-25e5-5e1297b09953&amp;rnd=79821</v>
       </c>
       <c r="C41" t="str">
         <v>Image</v>
@@ -1662,7 +1662,7 @@
         <v>1</v>
       </c>
       <c r="B42" t="str">
-        <v>https://speech18.leseweb.dk/rawfiles/extern2.min.js</v>
+        <v>https://speech1.leseweb.dk/rawfiles/extern2.min.js</v>
       </c>
       <c r="C42" t="str">
         <v>Script</v>
@@ -1688,7 +1688,7 @@
         <v>1</v>
       </c>
       <c r="B43" t="str">
-        <v>https://speech18.leseweb.dk/rawfiles/vfact2.min.js</v>
+        <v>https://speech1.leseweb.dk/rawfiles/vfact2.min.js</v>
       </c>
       <c r="C43" t="str">
         <v>Script</v>
@@ -1697,16 +1697,16 @@
         <v>text/javascript</v>
       </c>
       <c r="E43">
-        <v>13135</v>
+        <v>13134</v>
       </c>
       <c r="F43">
-        <v>42732</v>
+        <v>42731</v>
       </c>
       <c r="G43">
-        <v>0.0038198287549999995</v>
+        <v>0.0038195379419999997</v>
       </c>
       <c r="H43">
-        <v>0.005031774189000001</v>
+        <v>0.005031391107600001</v>
       </c>
     </row>
     <row r="44">
@@ -1749,16 +1749,16 @@
         <v>image/vnd.microsoft.icon</v>
       </c>
       <c r="E45">
-        <v>15400</v>
+        <v>15382</v>
       </c>
       <c r="F45">
         <v>15086</v>
       </c>
       <c r="G45">
-        <v>0.004478520199999999</v>
+        <v>0.004473285565999999</v>
       </c>
       <c r="H45">
-        <v>0.005899453560000001</v>
+        <v>0.005892558094800001</v>
       </c>
     </row>
     <row r="46">
@@ -1853,16 +1853,16 @@
         <v>text/html</v>
       </c>
       <c r="E49">
-        <v>31224</v>
+        <v>31259</v>
       </c>
       <c r="F49">
-        <v>154091</v>
+        <v>153997</v>
       </c>
       <c r="G49">
-        <v>0.009080345111999998</v>
+        <v>0.009090523567</v>
       </c>
       <c r="H49">
-        <v>0.011961333633600002</v>
+        <v>0.0119747414826</v>
       </c>
     </row>
     <row r="50">
@@ -1931,16 +1931,16 @@
         <v>text/css</v>
       </c>
       <c r="E52">
-        <v>60289</v>
+        <v>60288</v>
       </c>
       <c r="F52">
         <v>599332</v>
       </c>
       <c r="G52">
-        <v>0.017532824957</v>
+        <v>0.017532534144</v>
       </c>
       <c r="H52">
-        <v>0.023095594524600003</v>
+        <v>0.023095211443200002</v>
       </c>
     </row>
     <row r="53">
@@ -1957,16 +1957,16 @@
         <v>text/css</v>
       </c>
       <c r="E53">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F53">
         <v>578</v>
       </c>
       <c r="G53">
-        <v>0.000171870483</v>
+        <v>0.00017157967</v>
       </c>
       <c r="H53">
-        <v>0.00022640110740000002</v>
+        <v>0.00022601802599999998</v>
       </c>
     </row>
     <row r="54">
@@ -2009,16 +2009,16 @@
         <v>text/css</v>
       </c>
       <c r="E55">
-        <v>3484</v>
+        <v>3483</v>
       </c>
       <c r="F55">
         <v>12189</v>
       </c>
       <c r="G55">
-        <v>0.0010131924919999998</v>
+        <v>0.001012901679</v>
       </c>
       <c r="H55">
-        <v>0.0013346555976</v>
+        <v>0.0013342725162000001</v>
       </c>
     </row>
     <row r="56">
@@ -2061,16 +2061,16 @@
         <v>text/javascript</v>
       </c>
       <c r="E57">
-        <v>89995</v>
+        <v>31287</v>
       </c>
       <c r="F57">
         <v>89664</v>
       </c>
       <c r="G57">
-        <v>0.026171715934999996</v>
+        <v>0.009098666330999998</v>
       </c>
       <c r="H57">
-        <v>0.034475410593</v>
+        <v>0.011985467761800001</v>
       </c>
     </row>
     <row r="58">
@@ -2104,7 +2104,7 @@
         <v>2</v>
       </c>
       <c r="B59" t="str">
-        <v>https://www.as.kommune.no/css/cpcommon.css?v=20251110</v>
+        <v>https://www.as.kommune.no/css/cpcommon.css?v=20251114</v>
       </c>
       <c r="C59" t="str">
         <v>Stylesheet</v>
@@ -2234,7 +2234,7 @@
         <v>2</v>
       </c>
       <c r="B64" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464727.2703.jkzawaluazsnml/660f450/0_5464727.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5465224.2703.77iqmqbjzltqtt/660f450/0_5465224.jpg</v>
       </c>
       <c r="C64" t="str">
         <v>Image</v>
@@ -2243,16 +2243,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E64">
-        <v>43748</v>
+        <v>41979</v>
       </c>
       <c r="F64">
-        <v>43380</v>
+        <v>41611</v>
       </c>
       <c r="G64">
-        <v>0.012722487123999999</v>
+        <v>0.012208038926999999</v>
       </c>
       <c r="H64">
-        <v>0.0167590450872</v>
+        <v>0.0160813740906</v>
       </c>
     </row>
     <row r="65">
@@ -2260,7 +2260,7 @@
         <v>2</v>
       </c>
       <c r="B65" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464715.2703.bpjzpuutzsii7i/660f450/0_5464715.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5308658.2703.aabaszjkaptpbb/660f450/0_5308658.jpg</v>
       </c>
       <c r="C65" t="str">
         <v>Image</v>
@@ -2269,16 +2269,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E65">
-        <v>66510</v>
+        <v>29106</v>
       </c>
       <c r="F65">
-        <v>66142</v>
+        <v>28738</v>
       </c>
       <c r="G65">
-        <v>0.019341972629999996</v>
+        <v>0.008464403177999999</v>
       </c>
       <c r="H65">
-        <v>0.025478743914000006</v>
+        <v>0.011149967228399999</v>
       </c>
     </row>
     <row r="66">
@@ -2286,25 +2286,25 @@
         <v>2</v>
       </c>
       <c r="B66" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464624.2703.miqqnuwwzzswqt/660f450/0_5464624.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5464874.2703.jblqzspatzuwkt/660f450/0_5464874.png</v>
       </c>
       <c r="C66" t="str">
         <v>Image</v>
       </c>
       <c r="D66" t="str">
-        <v>image/jpeg</v>
+        <v>image/png</v>
       </c>
       <c r="E66">
-        <v>43585</v>
+        <v>159684</v>
       </c>
       <c r="F66">
-        <v>43217</v>
+        <v>159316</v>
       </c>
       <c r="G66">
-        <v>0.012675084605</v>
+        <v>0.046438183092</v>
       </c>
       <c r="H66">
-        <v>0.016696602819</v>
+        <v>0.061171970277600005</v>
       </c>
     </row>
     <row r="67">
@@ -2312,7 +2312,7 @@
         <v>2</v>
       </c>
       <c r="B67" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464266.2703.tkumwmpjsjqllz/660f450/0_5464266.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5464727.2703.jkzawaluazsnml/660f450/0_5464727.jpg</v>
       </c>
       <c r="C67" t="str">
         <v>Image</v>
@@ -2321,16 +2321,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E67">
-        <v>50396</v>
+        <v>43748</v>
       </c>
       <c r="F67">
-        <v>50028</v>
+        <v>43380</v>
       </c>
       <c r="G67">
-        <v>0.014655811947999997</v>
+        <v>0.012722487123999999</v>
       </c>
       <c r="H67">
-        <v>0.019305770234400003</v>
+        <v>0.0167590450872</v>
       </c>
     </row>
     <row r="68">
@@ -2338,7 +2338,7 @@
         <v>2</v>
       </c>
       <c r="B68" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464265.2703.jakzlmuauupstp/660f450/0_5464265.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5464715.2703.bpjzpuutzsii7i/660f450/0_5464715.jpg</v>
       </c>
       <c r="C68" t="str">
         <v>Image</v>
@@ -2347,16 +2347,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E68">
-        <v>40520</v>
+        <v>66510</v>
       </c>
       <c r="F68">
-        <v>40152</v>
+        <v>66142</v>
       </c>
       <c r="G68">
-        <v>0.011783742759999999</v>
+        <v>0.019341972629999996</v>
       </c>
       <c r="H68">
-        <v>0.015522458328000002</v>
+        <v>0.025478743914000006</v>
       </c>
     </row>
     <row r="69">
@@ -2364,7 +2364,7 @@
         <v>2</v>
       </c>
       <c r="B69" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464165.2703.njinmipitzqa7i/660f450/0_5464165.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5464624.2703.miqqnuwwzzswqt/660f450/0_5464624.jpg</v>
       </c>
       <c r="C69" t="str">
         <v>Image</v>
@@ -2373,16 +2373,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E69">
-        <v>61382</v>
+        <v>43585</v>
       </c>
       <c r="F69">
-        <v>61014</v>
+        <v>43217</v>
       </c>
       <c r="G69">
-        <v>0.017850683565999996</v>
+        <v>0.012675084605</v>
       </c>
       <c r="H69">
-        <v>0.023514302494800004</v>
+        <v>0.016696602819</v>
       </c>
     </row>
     <row r="70">
@@ -2390,7 +2390,7 @@
         <v>2</v>
       </c>
       <c r="B70" t="str">
-        <v>https://media.newmindmedia.com/TellUs/image/?file=Bilde_av_plakat_4__2060226217.png&amp;dh=515&amp;dw=350</v>
+        <v>https://media.newmindmedia.com/TellUs/image/?file=Logo_A_s_JPG_2__1509348857.jpg&amp;dh=139&amp;dw=350</v>
       </c>
       <c r="C70" t="str">
         <v>Image</v>
@@ -2399,16 +2399,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E70">
-        <v>47261</v>
+        <v>8692</v>
       </c>
       <c r="F70">
-        <v>46939</v>
+        <v>8414</v>
       </c>
       <c r="G70">
-        <v>0.013744113192999998</v>
+        <v>0.0025277465959999998</v>
       </c>
       <c r="H70">
-        <v>0.018104810045400002</v>
+        <v>0.0033297435288000008</v>
       </c>
     </row>
     <row r="71">
@@ -2416,7 +2416,7 @@
         <v>2</v>
       </c>
       <c r="B71" t="str">
-        <v>https://media.newmindmedia.com/TellUs/image/?file=Vintersykkelfest_233473079.jpg&amp;dh=350&amp;dw=350</v>
+        <v>https://media.newmindmedia.com/TellUs/image/?file=F322105710F853B986D230AE1BF4B921F4143F8C_944246711.jpg&amp;dh=361&amp;dw=350</v>
       </c>
       <c r="C71" t="str">
         <v>Image</v>
@@ -2425,16 +2425,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E71">
-        <v>33726</v>
+        <v>26125</v>
       </c>
       <c r="F71">
-        <v>33422</v>
+        <v>25830</v>
       </c>
       <c r="G71">
-        <v>0.009807959237999998</v>
+        <v>0.007597489624999999</v>
       </c>
       <c r="H71">
-        <v>0.0129198032964</v>
+        <v>0.010008001575000001</v>
       </c>
     </row>
     <row r="72">
@@ -2442,7 +2442,7 @@
         <v>2</v>
       </c>
       <c r="B72" t="str">
-        <v>https://media.newmindmedia.com/TellUs/image/?file=KRED_1794052439.jpg&amp;dh=197&amp;dw=350</v>
+        <v>https://media.newmindmedia.com/TellUs/image/?file=1B4C24285867A1B7CDF44DF0370ACB0E18D8485A_1352853877.jpg&amp;dh=469&amp;dw=350</v>
       </c>
       <c r="C72" t="str">
         <v>Image</v>
@@ -2451,16 +2451,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E72">
-        <v>12203</v>
+        <v>22591</v>
       </c>
       <c r="F72">
-        <v>11924</v>
+        <v>22296</v>
       </c>
       <c r="G72">
-        <v>0.0035487910389999993</v>
+        <v>0.006569756482999999</v>
       </c>
       <c r="H72">
-        <v>0.0046747423242</v>
+        <v>0.008654191907400001</v>
       </c>
     </row>
     <row r="73">
@@ -2477,16 +2477,16 @@
         <v>application/javascript</v>
       </c>
       <c r="E73">
-        <v>13687</v>
+        <v>13686</v>
       </c>
       <c r="F73">
         <v>43534</v>
       </c>
       <c r="G73">
-        <v>0.0039803575309999995</v>
+        <v>0.003980066717999999</v>
       </c>
       <c r="H73">
-        <v>0.0052432351218</v>
+        <v>0.005242852040400001</v>
       </c>
     </row>
     <row r="74">
@@ -2786,16 +2786,16 @@
         <v>text/html</v>
       </c>
       <c r="E85">
-        <v>4040</v>
+        <v>4042</v>
       </c>
       <c r="F85">
         <v>15600</v>
       </c>
       <c r="G85">
-        <v>0.0011748845199999998</v>
+        <v>0.0011754661459999999</v>
       </c>
       <c r="H85">
-        <v>0.0015476488560000005</v>
+        <v>0.0015484150188</v>
       </c>
     </row>
     <row r="86">
@@ -2855,7 +2855,7 @@
         <v>2</v>
       </c>
       <c r="B88" t="str">
-        <v>https://6002261.global.siteimproveanalytics.io/image.aspx?url=https%3A%2F%2Fwww.as.kommune.no%2F&amp;title=Forside%20-%20%C3%85S%20KOMMUNE&amp;res=412x823&amp;accountid=6002261&amp;rt=231&amp;prev=f6c38f73-fce3-0a1a-525d-080eaef50344&amp;luid=4c8def7b-134a-817a-1d80-d837a0696b7b&amp;rnd=82618</v>
+        <v>https://6002261.global.siteimproveanalytics.io/image.aspx?url=https%3A%2F%2Fwww.as.kommune.no%2F&amp;title=Forside%20-%20%C3%85S%20KOMMUNE&amp;res=412x823&amp;accountid=6002261&amp;rt=239&amp;prev=249c62a5-4f23-2ba9-ccc3-f1777424a4f6&amp;luid=4cfe65c7-ed32-fbcf-43ef-61fd92270eea&amp;rnd=35514</v>
       </c>
       <c r="C88" t="str">
         <v>Image</v>
@@ -2881,7 +2881,7 @@
         <v>2</v>
       </c>
       <c r="B89" t="str">
-        <v>https://speech1.leseweb.dk/rawfiles/extern2.min.js</v>
+        <v>https://speech4.leseweb.dk/rawfiles/extern2.min.js</v>
       </c>
       <c r="C89" t="str">
         <v>Script</v>
@@ -2907,7 +2907,7 @@
         <v>2</v>
       </c>
       <c r="B90" t="str">
-        <v>https://speech1.leseweb.dk/rawfiles/vfact2.min.js</v>
+        <v>https://speech4.leseweb.dk/rawfiles/vfact2.min.js</v>
       </c>
       <c r="C90" t="str">
         <v>Script</v>
@@ -2916,16 +2916,16 @@
         <v>text/javascript</v>
       </c>
       <c r="E90">
-        <v>13134</v>
+        <v>13135</v>
       </c>
       <c r="F90">
         <v>42731</v>
       </c>
       <c r="G90">
-        <v>0.0038195379419999997</v>
+        <v>0.0038198287549999995</v>
       </c>
       <c r="H90">
-        <v>0.005031391107600001</v>
+        <v>0.005031774189000001</v>
       </c>
     </row>
     <row r="91">
@@ -3072,16 +3072,16 @@
         <v>text/html</v>
       </c>
       <c r="E96">
-        <v>31232</v>
+        <v>31260</v>
       </c>
       <c r="F96">
-        <v>154091</v>
+        <v>153997</v>
       </c>
       <c r="G96">
-        <v>0.009082671615999998</v>
+        <v>0.00909081438</v>
       </c>
       <c r="H96">
-        <v>0.011964398284800002</v>
+        <v>0.011975124564000001</v>
       </c>
     </row>
     <row r="97">
@@ -3150,16 +3150,16 @@
         <v>text/css</v>
       </c>
       <c r="E99">
-        <v>60289</v>
+        <v>60279</v>
       </c>
       <c r="F99">
         <v>599332</v>
       </c>
       <c r="G99">
-        <v>0.017532824957</v>
+        <v>0.017529916826999996</v>
       </c>
       <c r="H99">
-        <v>0.023095594524600003</v>
+        <v>0.0230917637106</v>
       </c>
     </row>
     <row r="100">
@@ -3176,16 +3176,16 @@
         <v>text/css</v>
       </c>
       <c r="E100">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F100">
         <v>578</v>
       </c>
       <c r="G100">
-        <v>0.000171870483</v>
+        <v>0.00017157967</v>
       </c>
       <c r="H100">
-        <v>0.00022640110740000002</v>
+        <v>0.00022601802599999998</v>
       </c>
     </row>
     <row r="101">
@@ -3202,16 +3202,16 @@
         <v>text/css</v>
       </c>
       <c r="E101">
-        <v>2226</v>
+        <v>2227</v>
       </c>
       <c r="F101">
         <v>17559</v>
       </c>
       <c r="G101">
-        <v>0.0006473497379999998</v>
+        <v>0.0006476405509999999</v>
       </c>
       <c r="H101">
-        <v>0.0008527391964</v>
+        <v>0.0008531222778000001</v>
       </c>
     </row>
     <row r="102">
@@ -3228,16 +3228,16 @@
         <v>text/css</v>
       </c>
       <c r="E102">
-        <v>3484</v>
+        <v>3483</v>
       </c>
       <c r="F102">
         <v>12189</v>
       </c>
       <c r="G102">
-        <v>0.0010131924919999998</v>
+        <v>0.001012901679</v>
       </c>
       <c r="H102">
-        <v>0.0013346555976</v>
+        <v>0.0013342725162000001</v>
       </c>
     </row>
     <row r="103">
@@ -3280,16 +3280,16 @@
         <v>text/javascript</v>
       </c>
       <c r="E104">
-        <v>89995</v>
+        <v>31287</v>
       </c>
       <c r="F104">
         <v>89664</v>
       </c>
       <c r="G104">
-        <v>0.026171715934999996</v>
+        <v>0.009098666330999998</v>
       </c>
       <c r="H104">
-        <v>0.034475410593</v>
+        <v>0.011985467761800001</v>
       </c>
     </row>
     <row r="105">
@@ -3323,7 +3323,7 @@
         <v>3</v>
       </c>
       <c r="B106" t="str">
-        <v>https://www.as.kommune.no/css/cpcommon.css?v=20251110</v>
+        <v>https://www.as.kommune.no/css/cpcommon.css?v=20251114</v>
       </c>
       <c r="C106" t="str">
         <v>Stylesheet</v>
@@ -3453,7 +3453,7 @@
         <v>3</v>
       </c>
       <c r="B111" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464727.2703.jkzawaluazsnml/660f450/0_5464727.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5465224.2703.77iqmqbjzltqtt/660f450/0_5465224.jpg</v>
       </c>
       <c r="C111" t="str">
         <v>Image</v>
@@ -3462,16 +3462,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E111">
-        <v>43748</v>
+        <v>41979</v>
       </c>
       <c r="F111">
-        <v>43380</v>
+        <v>41611</v>
       </c>
       <c r="G111">
-        <v>0.012722487123999999</v>
+        <v>0.012208038926999999</v>
       </c>
       <c r="H111">
-        <v>0.0167590450872</v>
+        <v>0.0160813740906</v>
       </c>
     </row>
     <row r="112">
@@ -3479,7 +3479,7 @@
         <v>3</v>
       </c>
       <c r="B112" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464715.2703.bpjzpuutzsii7i/660f450/0_5464715.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5308658.2703.aabaszjkaptpbb/660f450/0_5308658.jpg</v>
       </c>
       <c r="C112" t="str">
         <v>Image</v>
@@ -3488,16 +3488,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E112">
-        <v>66510</v>
+        <v>29106</v>
       </c>
       <c r="F112">
-        <v>66142</v>
+        <v>28738</v>
       </c>
       <c r="G112">
-        <v>0.019341972629999996</v>
+        <v>0.008464403177999999</v>
       </c>
       <c r="H112">
-        <v>0.025478743914000006</v>
+        <v>0.011149967228399999</v>
       </c>
     </row>
     <row r="113">
@@ -3505,25 +3505,25 @@
         <v>3</v>
       </c>
       <c r="B113" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464624.2703.miqqnuwwzzswqt/660f450/0_5464624.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5464874.2703.jblqzspatzuwkt/660f450/0_5464874.png</v>
       </c>
       <c r="C113" t="str">
         <v>Image</v>
       </c>
       <c r="D113" t="str">
-        <v>image/jpeg</v>
+        <v>image/png</v>
       </c>
       <c r="E113">
-        <v>43585</v>
+        <v>159684</v>
       </c>
       <c r="F113">
-        <v>43217</v>
+        <v>159316</v>
       </c>
       <c r="G113">
-        <v>0.012675084605</v>
+        <v>0.046438183092</v>
       </c>
       <c r="H113">
-        <v>0.016696602819</v>
+        <v>0.061171970277600005</v>
       </c>
     </row>
     <row r="114">
@@ -3531,7 +3531,7 @@
         <v>3</v>
       </c>
       <c r="B114" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464266.2703.tkumwmpjsjqllz/660f450/0_5464266.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5464727.2703.jkzawaluazsnml/660f450/0_5464727.jpg</v>
       </c>
       <c r="C114" t="str">
         <v>Image</v>
@@ -3540,16 +3540,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E114">
-        <v>50396</v>
+        <v>43748</v>
       </c>
       <c r="F114">
-        <v>50028</v>
+        <v>43380</v>
       </c>
       <c r="G114">
-        <v>0.014655811947999997</v>
+        <v>0.012722487123999999</v>
       </c>
       <c r="H114">
-        <v>0.019305770234400003</v>
+        <v>0.0167590450872</v>
       </c>
     </row>
     <row r="115">
@@ -3557,7 +3557,7 @@
         <v>3</v>
       </c>
       <c r="B115" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464265.2703.jakzlmuauupstp/660f450/0_5464265.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5464715.2703.bpjzpuutzsii7i/660f450/0_5464715.jpg</v>
       </c>
       <c r="C115" t="str">
         <v>Image</v>
@@ -3566,16 +3566,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E115">
-        <v>40520</v>
+        <v>66510</v>
       </c>
       <c r="F115">
-        <v>40152</v>
+        <v>66142</v>
       </c>
       <c r="G115">
-        <v>0.011783742759999999</v>
+        <v>0.019341972629999996</v>
       </c>
       <c r="H115">
-        <v>0.015522458328000002</v>
+        <v>0.025478743914000006</v>
       </c>
     </row>
     <row r="116">
@@ -3583,7 +3583,7 @@
         <v>3</v>
       </c>
       <c r="B116" t="str">
-        <v>https://img3.custompublish.com/getfile.php/5464165.2703.njinmipitzqa7i/660f450/0_5464165.jpg</v>
+        <v>https://img3.custompublish.com/getfile.php/5464624.2703.miqqnuwwzzswqt/660f450/0_5464624.jpg</v>
       </c>
       <c r="C116" t="str">
         <v>Image</v>
@@ -3592,16 +3592,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E116">
-        <v>61382</v>
+        <v>43585</v>
       </c>
       <c r="F116">
-        <v>61014</v>
+        <v>43217</v>
       </c>
       <c r="G116">
-        <v>0.017850683565999996</v>
+        <v>0.012675084605</v>
       </c>
       <c r="H116">
-        <v>0.023514302494800004</v>
+        <v>0.016696602819</v>
       </c>
     </row>
     <row r="117">
@@ -3609,7 +3609,7 @@
         <v>3</v>
       </c>
       <c r="B117" t="str">
-        <v>https://media.newmindmedia.com/TellUs/image/?file=Bilde_av_plakat_4__2060226217.png&amp;dh=515&amp;dw=350</v>
+        <v>https://media.newmindmedia.com/TellUs/image/?file=Logo_A_s_JPG_2__1509348857.jpg&amp;dh=139&amp;dw=350</v>
       </c>
       <c r="C117" t="str">
         <v>Image</v>
@@ -3618,16 +3618,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E117">
-        <v>47261</v>
+        <v>8692</v>
       </c>
       <c r="F117">
-        <v>46939</v>
+        <v>8414</v>
       </c>
       <c r="G117">
-        <v>0.013744113192999998</v>
+        <v>0.0025277465959999998</v>
       </c>
       <c r="H117">
-        <v>0.018104810045400002</v>
+        <v>0.0033297435288000008</v>
       </c>
     </row>
     <row r="118">
@@ -3635,7 +3635,7 @@
         <v>3</v>
       </c>
       <c r="B118" t="str">
-        <v>https://media.newmindmedia.com/TellUs/image/?file=Vintersykkelfest_233473079.jpg&amp;dh=350&amp;dw=350</v>
+        <v>https://media.newmindmedia.com/TellUs/image/?file=F322105710F853B986D230AE1BF4B921F4143F8C_944246711.jpg&amp;dh=361&amp;dw=350</v>
       </c>
       <c r="C118" t="str">
         <v>Image</v>
@@ -3644,16 +3644,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E118">
-        <v>33726</v>
+        <v>26125</v>
       </c>
       <c r="F118">
-        <v>33422</v>
+        <v>25830</v>
       </c>
       <c r="G118">
-        <v>0.009807959237999998</v>
+        <v>0.007597489624999999</v>
       </c>
       <c r="H118">
-        <v>0.0129198032964</v>
+        <v>0.010008001575000001</v>
       </c>
     </row>
     <row r="119">
@@ -3661,7 +3661,7 @@
         <v>3</v>
       </c>
       <c r="B119" t="str">
-        <v>https://media.newmindmedia.com/TellUs/image/?file=KRED_1794052439.jpg&amp;dh=197&amp;dw=350</v>
+        <v>https://media.newmindmedia.com/TellUs/image/?file=1B4C24285867A1B7CDF44DF0370ACB0E18D8485A_1352853877.jpg&amp;dh=469&amp;dw=350</v>
       </c>
       <c r="C119" t="str">
         <v>Image</v>
@@ -3670,16 +3670,16 @@
         <v>image/jpeg</v>
       </c>
       <c r="E119">
-        <v>12203</v>
+        <v>22591</v>
       </c>
       <c r="F119">
-        <v>11924</v>
+        <v>22296</v>
       </c>
       <c r="G119">
-        <v>0.0035487910389999993</v>
+        <v>0.006569756482999999</v>
       </c>
       <c r="H119">
-        <v>0.0046747423242</v>
+        <v>0.008654191907400001</v>
       </c>
     </row>
     <row r="120">
@@ -3696,16 +3696,16 @@
         <v>application/javascript</v>
       </c>
       <c r="E120">
-        <v>13695</v>
+        <v>13689</v>
       </c>
       <c r="F120">
         <v>43534</v>
       </c>
       <c r="G120">
-        <v>0.003982684035</v>
+        <v>0.003980939156999999</v>
       </c>
       <c r="H120">
-        <v>0.005246299773</v>
+        <v>0.0052440012846000006</v>
       </c>
     </row>
     <row r="121">
@@ -4005,16 +4005,16 @@
         <v>text/html</v>
       </c>
       <c r="E132">
-        <v>4039</v>
+        <v>4040</v>
       </c>
       <c r="F132">
         <v>15600</v>
       </c>
       <c r="G132">
-        <v>0.0011745937069999998</v>
+        <v>0.0011748845199999998</v>
       </c>
       <c r="H132">
-        <v>0.0015472657746</v>
+        <v>0.0015476488560000005</v>
       </c>
     </row>
     <row r="133">
@@ -4074,7 +4074,7 @@
         <v>3</v>
       </c>
       <c r="B135" t="str">
-        <v>https://6002261.global.siteimproveanalytics.io/image.aspx?url=https%3A%2F%2Fwww.as.kommune.no%2F&amp;title=Forside%20-%20%C3%85S%20KOMMUNE&amp;res=412x823&amp;accountid=6002261&amp;rt=222&amp;prev=fb38d387-19b7-1020-f758-4bda050c959b&amp;luid=1a6e613b-7576-9c0f-2857-30b335db8aa7&amp;rnd=27028</v>
+        <v>https://6002261.global.siteimproveanalytics.io/image.aspx?url=https%3A%2F%2Fwww.as.kommune.no%2F&amp;title=Forside%20-%20%C3%85S%20KOMMUNE&amp;res=412x823&amp;accountid=6002261&amp;rt=256&amp;prev=1d237f02-7626-d963-0ee0-deac7d4614aa&amp;luid=ecc64171-4d8d-5205-e743-ddd501cdccec&amp;rnd=27426</v>
       </c>
       <c r="C135" t="str">
         <v>Image</v>
@@ -4100,7 +4100,7 @@
         <v>3</v>
       </c>
       <c r="B136" t="str">
-        <v>https://speech21.leseweb.dk/rawfiles/extern2.min.js</v>
+        <v>https://speech11.leseweb.dk/rawfiles/extern2.min.js</v>
       </c>
       <c r="C136" t="str">
         <v>Script</v>
@@ -4126,7 +4126,7 @@
         <v>3</v>
       </c>
       <c r="B137" t="str">
-        <v>https://speech21.leseweb.dk/rawfiles/vfact2.min.js</v>
+        <v>https://speech11.leseweb.dk/rawfiles/vfact2.min.js</v>
       </c>
       <c r="C137" t="str">
         <v>Script</v>
@@ -4161,16 +4161,16 @@
         <v>application/octet-stream</v>
       </c>
       <c r="E138">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F138">
         <v>291</v>
       </c>
       <c r="G138">
-        <v>0.00018379381599999999</v>
+        <v>0.00018408462899999997</v>
       </c>
       <c r="H138">
-        <v>0.0002421074448</v>
+        <v>0.0002424905262</v>
       </c>
     </row>
     <row r="139">
@@ -4313,10 +4313,10 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>93687</v>
+        <v>93777</v>
       </c>
       <c r="D2">
-        <v>462272</v>
+        <v>461990</v>
       </c>
     </row>
     <row r="3">
@@ -4327,7 +4327,7 @@
         <v>33</v>
       </c>
       <c r="C3">
-        <v>272028</v>
+        <v>272012</v>
       </c>
       <c r="D3">
         <v>2222016</v>
@@ -4341,10 +4341,10 @@
         <v>33</v>
       </c>
       <c r="C4">
-        <v>1941343</v>
+        <v>1765199</v>
       </c>
       <c r="D4">
-        <v>2603817</v>
+        <v>2603814</v>
       </c>
     </row>
     <row r="5">
@@ -4355,10 +4355,10 @@
         <v>54</v>
       </c>
       <c r="C5">
-        <v>2017386</v>
+        <v>2145444</v>
       </c>
       <c r="D5">
-        <v>2005503</v>
+        <v>2133681</v>
       </c>
     </row>
     <row r="6">
@@ -4397,7 +4397,7 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>12119</v>
+        <v>12121</v>
       </c>
       <c r="D8">
         <v>46800</v>
@@ -4411,7 +4411,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>1898</v>
+        <v>1899</v>
       </c>
       <c r="D9">
         <v>873</v>
@@ -4425,7 +4425,7 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <v>46164</v>
+        <v>46146</v>
       </c>
       <c r="D10">
         <v>45258</v>
@@ -4464,13 +4464,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1537160</v>
+        <v>1521124</v>
       </c>
       <c r="C2">
-        <v>0.4470261110799999</v>
+        <v>0.4423626338119999</v>
       </c>
       <c r="D2">
-        <v>0.5888574048240002</v>
+        <v>0.5827143114936001</v>
       </c>
     </row>
     <row r="3">
@@ -4478,13 +4478,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1537129</v>
+        <v>1521144</v>
       </c>
       <c r="C3">
-        <v>0.44701709587699995</v>
+        <v>0.44236845007199993</v>
       </c>
       <c r="D3">
-        <v>0.5888455293006001</v>
+        <v>0.5827219731216001</v>
       </c>
     </row>
     <row r="4">
@@ -4492,13 +4492,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1537136</v>
+        <v>1521130</v>
       </c>
       <c r="C4">
-        <v>0.44701913156799994</v>
+        <v>0.44236437868999995</v>
       </c>
       <c r="D4">
-        <v>0.5888482108704</v>
+        <v>0.582716609982</v>
       </c>
     </row>
     <row r="5">
@@ -4506,13 +4506,13 @@
         <v>median</v>
       </c>
       <c r="B5">
-        <v>1537136</v>
+        <v>1521130</v>
       </c>
       <c r="C5">
-        <v>0.44701913156799994</v>
+        <v>0.44236437868999995</v>
       </c>
       <c r="D5">
-        <v>0.5888482108704</v>
+        <v>0.582716609982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>